<commit_message>
:recycle: Dot to comma prompt consistency improvement
</commit_message>
<xml_diff>
--- a/assets/docs_output/Teste Execução - 18_12_2024 - Test_Execution_data Template.xlsx
+++ b/assets/docs_output/Teste Execução - 18_12_2024 - Test_Execution_data Template.xlsx
@@ -19745,7 +19745,11 @@
       </c>
     </row>
     <row r="498">
-      <c r="A498" t="inlineStr"/>
+      <c r="A498" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
       <c r="B498" t="inlineStr"/>
       <c r="C498" t="inlineStr"/>
       <c r="D498" t="inlineStr">

</xml_diff>